<commit_message>
updated requirements - high level
</commit_message>
<xml_diff>
--- a/docs/Architecture/High_Level_Requirements.xlsx
+++ b/docs/Architecture/High_Level_Requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/c_karagoz_tue_nl/Documents/Documents/GitHub/AutonomousReferee/docs/Architecture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSD2021_AutoRef\AutonomousReferee\docs\Architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{DA2E0490-2C8A-4FE5-AB71-6A07DA039F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B044514-37DD-4F60-9473-61D7149AF61A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1925B7B-7BBE-4A7F-A96A-373277254A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="MC" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
   <si>
     <t>Exercize requirements concerning system (scope): AutoRef system</t>
   </si>
@@ -598,22 +598,22 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -629,7 +629,7 @@
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -645,7 +645,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -683,7 +683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -721,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -797,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -808,7 +808,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -846,7 +846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -884,7 +884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -922,7 +922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -960,7 +960,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -998,7 +998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -1089,28 +1089,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB766EA-E4CB-470E-BE50-5F8372C02EE6}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" style="2"/>
-    <col min="2" max="2" width="19.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="8.5703125" style="2"/>
+    <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1126,7 @@
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
@@ -1142,7 +1142,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1180,460 +1180,108 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:12" s="3" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="2">
-        <v>4</v>
-      </c>
-      <c r="H16" s="2">
-        <v>5</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1</v>
-      </c>
-      <c r="J16" s="2">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1</v>
-      </c>
-      <c r="L16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="2">
-        <v>3</v>
-      </c>
-      <c r="H17" s="2">
-        <v>5</v>
-      </c>
-      <c r="I17" s="2">
-        <v>1</v>
-      </c>
-      <c r="J17" s="2">
-        <v>1</v>
-      </c>
-      <c r="K17" s="2">
-        <v>1</v>
-      </c>
-      <c r="L17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="2">
-        <v>4</v>
-      </c>
-      <c r="H18" s="2">
-        <v>3</v>
-      </c>
-      <c r="I18" s="2">
-        <v>1</v>
-      </c>
-      <c r="J18" s="2">
-        <v>1</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1</v>
-      </c>
-      <c r="L18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="2">
-        <v>5</v>
-      </c>
-      <c r="H21" s="2">
-        <v>4</v>
-      </c>
-      <c r="I21" s="2">
-        <v>5</v>
-      </c>
-      <c r="J21" s="2">
-        <v>5</v>
-      </c>
-      <c r="K21" s="2">
-        <v>5</v>
-      </c>
-      <c r="L21" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22" s="2">
-        <v>4</v>
-      </c>
-      <c r="H22" s="2">
-        <v>4</v>
-      </c>
-      <c r="I22" s="2">
-        <v>4</v>
-      </c>
-      <c r="J22" s="2">
-        <v>4</v>
-      </c>
-      <c r="K22" s="2">
-        <v>3</v>
-      </c>
-      <c r="L22" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="2">
-        <v>5</v>
-      </c>
-      <c r="H23" s="2">
-        <v>5</v>
-      </c>
-      <c r="I23" s="2">
-        <v>5</v>
-      </c>
-      <c r="J23" s="2">
-        <v>5</v>
-      </c>
-      <c r="K23" s="2">
-        <v>5</v>
-      </c>
-      <c r="L23" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="2">
-        <v>5</v>
-      </c>
-      <c r="H24" s="2">
-        <v>5</v>
-      </c>
-      <c r="I24" s="2">
-        <v>5</v>
-      </c>
-      <c r="J24" s="2">
-        <v>5</v>
-      </c>
-      <c r="K24" s="2">
-        <v>4</v>
-      </c>
-      <c r="L24" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G26" s="2">
-        <v>3</v>
-      </c>
-      <c r="H26" s="2">
-        <v>3</v>
-      </c>
-      <c r="I26" s="2">
-        <v>3</v>
-      </c>
-      <c r="J26" s="2">
-        <v>4</v>
-      </c>
-      <c r="K26" s="2">
-        <v>5</v>
-      </c>
-      <c r="L26" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27" s="2">
-        <v>3</v>
-      </c>
-      <c r="H27" s="2">
-        <v>3</v>
-      </c>
-      <c r="I27" s="2">
-        <v>4</v>
-      </c>
-      <c r="J27" s="2">
-        <v>4</v>
-      </c>
-      <c r="K27" s="2">
-        <v>5</v>
-      </c>
-      <c r="L27" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G28" s="2">
-        <v>4</v>
-      </c>
-      <c r="H28" s="2">
-        <v>4</v>
-      </c>
-      <c r="I28" s="2">
-        <v>3</v>
-      </c>
-      <c r="J28" s="2">
-        <v>3</v>
-      </c>
-      <c r="K28" s="2">
-        <v>5</v>
-      </c>
-      <c r="L28" s="2">
-        <v>5</v>
-      </c>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
requirements register filled with missing information
</commit_message>
<xml_diff>
--- a/docs/Architecture/High_Level_Requirements.xlsx
+++ b/docs/Architecture/High_Level_Requirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSD2021_AutoRef\AutonomousReferee\docs\Architecture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Referee\AutonomousReferee\docs\Architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1925B7B-7BBE-4A7F-A96A-373277254A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E236AC1-0827-42C1-8A94-5C587FC4622E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="77">
   <si>
     <t>Exercize requirements concerning system (scope): AutoRef system</t>
   </si>
@@ -208,19 +208,10 @@
     <t>The AutoRef shall cover the scenarios for the rule violations that were simulated by MSD 2020 batch. (As per the document XXXXX)</t>
   </si>
   <si>
-    <t>The AutoRef shall communicate the rule violations to the RefBox/human referee.</t>
-  </si>
-  <si>
-    <t>The AutoRef shall communicate the match related time details to the RefBox/human referee.</t>
-  </si>
-  <si>
     <t>The AutoRef shall log the rule violation incidents for evidence.</t>
   </si>
   <si>
     <t>The autonomous refereeing system(AutoRef) shall referee 5 minutes match with 2 vs 2 soccer robots.</t>
-  </si>
-  <si>
-    <t>The AutoRef rule violation decisions shall/should receive positive feedback from human referee.</t>
   </si>
   <si>
     <t>The AutoRef system shall be used as a developemnt platform for further improvements and enhancements by the upcoming MSD teams.
@@ -228,13 +219,61 @@
   </si>
   <si>
     <t>The AutoRef shall make decisions based on the position, role, time, and xxxxxx data received.</t>
+  </si>
+  <si>
+    <t>The AutoRef shall indicate the rule violations (to the RefBox/human referee).</t>
+  </si>
+  <si>
+    <t>The AutoRef shall inidcate the match related time details(to the RefBox/human referee).</t>
+  </si>
+  <si>
+    <t>5 minutes</t>
+  </si>
+  <si>
+    <t>extendability</t>
+  </si>
+  <si>
+    <t>decision maker</t>
+  </si>
+  <si>
+    <t>evidence</t>
+  </si>
+  <si>
+    <t>The AutoRef rule violation decisions should receive positive feedback from human referee.</t>
+  </si>
+  <si>
+    <t>positive feedback</t>
+  </si>
+  <si>
+    <t>Statisfaction Rene</t>
+  </si>
+  <si>
+    <t>Dissatisfaction Rene</t>
+  </si>
+  <si>
+    <t>Satifaction Erjen</t>
+  </si>
+  <si>
+    <t>Dissatisfaction Erjen</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Erjen?, Team</t>
+  </si>
+  <si>
+    <t>Rene</t>
+  </si>
+  <si>
+    <t>Erjen?,Team</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -247,6 +286,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -269,15 +319,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,54 +658,54 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -683,7 +743,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -721,7 +781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -759,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -797,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -808,7 +868,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -846,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -884,7 +944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -922,7 +982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -960,7 +1020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -998,7 +1058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1036,7 +1096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -1087,201 +1147,332 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB766EA-E4CB-470E-BE50-5F8372C02EE6}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="2"/>
-    <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="8.5546875" style="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    </row>
+    <row r="2" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2">
+        <v>4</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2">
+        <v>3</v>
+      </c>
+      <c r="I8" s="2">
+        <v>3</v>
+      </c>
+      <c r="J8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2">
+        <v>5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>5</v>
+      </c>
+      <c r="J9" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>8</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="2">
+        <v>3</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3</v>
+      </c>
+      <c r="I11" s="2">
+        <v>4</v>
+      </c>
+      <c r="J11" s="2">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1289,6 +1480,6 @@
     <mergeCell ref="A2:XFD2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>